<commit_message>
revert to old censored template
</commit_message>
<xml_diff>
--- a/inst/extdata/MassWateR_Censored_Template.xlsx
+++ b/inst/extdata/MassWateR_Censored_Template.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\proj\MassWateR\inst\extdata\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/9d8cbaaa4eaa566d/Documents/1 ACASAK/MassWateR/Design/Templates for users/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59968624-65A9-4B2C-95F9-CFB4FFFB5C22}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="29" documentId="8_{7581B32E-191D-471F-BE3B-DC8CDFE69C76}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00ECC116-CF47-46D4-A942-DCC7BF5804CE}"/>
   <bookViews>
-    <workbookView xWindow="29565" yWindow="2670" windowWidth="25170" windowHeight="11295" xr2:uid="{20339F69-97D7-4797-B0E4-E58661B4B2FE}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="13020" xr2:uid="{20339F69-97D7-4797-B0E4-E58661B4B2FE}"/>
   </bookViews>
   <sheets>
     <sheet name="Censored" sheetId="2" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="93" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="81">
   <si>
     <t>Parameter</t>
   </si>
@@ -394,7 +394,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -437,12 +437,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -758,13 +752,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C59ABFCD-EF8D-425C-92A4-3137E9EF3DBA}">
-  <dimension ref="A1:B9"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E11" sqref="E11"/>
+      <selection pane="bottomRight" activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -782,66 +776,26 @@
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="17" t="s">
-        <v>68</v>
-      </c>
-      <c r="B2" s="18">
-        <v>0</v>
+      <c r="A2" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="5">
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" s="5">
         <v>1</v>
-      </c>
-      <c r="B3" s="5">
-        <v>12</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="13" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B4" s="5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" s="13" t="s">
-        <v>49</v>
-      </c>
-      <c r="B5" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" s="13" t="s">
-        <v>65</v>
-      </c>
-      <c r="B6" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" s="13" t="s">
-        <v>3</v>
-      </c>
-      <c r="B7" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" s="13" t="s">
-        <v>12</v>
-      </c>
-      <c r="B8" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="13" t="s">
-        <v>8</v>
-      </c>
-      <c r="B9" s="5">
         <v>0</v>
       </c>
     </row>
@@ -855,7 +809,7 @@
           <x14:formula1>
             <xm:f>Values!$A$2:$A$68</xm:f>
           </x14:formula1>
-          <xm:sqref>A10:A1048576</xm:sqref>
+          <xm:sqref>A2:A1048576</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>

</xml_diff>